<commit_message>
Updates: setup_gui.py has been updated. Now the gui supports sheet selection and a destination directory. The gui also has a button to proceed which will return all the relevant information to the main program so that the main program can run.
Documentation finally added for excel_to_excel

Next steps: Documentation needed for setup_gui.py, re do gui from scratch
</commit_message>
<xml_diff>
--- a/Destination Workbook Testing/Destination.xlsx
+++ b/Destination Workbook Testing/Destination.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20391"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DE1388-ED91-495A-A42C-C28D52483445}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534038DE-DC49-470F-BCCC-B45302737F54}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,31 +20,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>I</t>
+    <t>Team Name</t>
   </si>
   <si>
-    <t>AM</t>
+    <t>Team Email</t>
   </si>
   <si>
-    <t>One</t>
+    <t>Team Phone</t>
   </si>
   <si>
-    <t>Who</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
+    <t>Team Budget</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,13 +46,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="22"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -73,8 +80,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -355,47 +363,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="26.5703125" customWidth="1"/>
+    <col min="3" max="4" width="25.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
First functional version of gui.py
Finished cell selection page

Created a backend loading screen where the excel files are being read and written to.
</commit_message>
<xml_diff>
--- a/Destination Workbook Testing/Destination.xlsx
+++ b/Destination Workbook Testing/Destination.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20392"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BB44A5-784D-4D7D-9676-D78151257F9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2FDED7E-7C13-4961-ABC4-152A91C9E95E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Team Name</t>
   </si>
@@ -32,54 +32,6 @@
   </si>
   <si>
     <t>Team Budget</t>
-  </si>
-  <si>
-    <t>Team A P1</t>
-  </si>
-  <si>
-    <t>Email A P1</t>
-  </si>
-  <si>
-    <t>Phone A P1</t>
-  </si>
-  <si>
-    <t>Budget A P1</t>
-  </si>
-  <si>
-    <t>Team A P2</t>
-  </si>
-  <si>
-    <t>Email A P2</t>
-  </si>
-  <si>
-    <t>Phone A P2</t>
-  </si>
-  <si>
-    <t>Budget A P2</t>
-  </si>
-  <si>
-    <t>Team B P1</t>
-  </si>
-  <si>
-    <t>Email B P1</t>
-  </si>
-  <si>
-    <t>Phone B P1</t>
-  </si>
-  <si>
-    <t>Budget B P1</t>
-  </si>
-  <si>
-    <t>Team B P2</t>
-  </si>
-  <si>
-    <t>Email B P2</t>
-  </si>
-  <si>
-    <t>Phone B P2</t>
-  </si>
-  <si>
-    <t>Budget B P2</t>
   </si>
 </sst>
 </file>
@@ -411,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D5" sqref="A2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,62 +389,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Sheet Validation and QOL improvements
Added a new page that is used to determine sheet completion

Added some documentation for building blocks. Now only gui.py needs documentation

Fixed the algorithm in excel_to_excel to work with sheet validation
</commit_message>
<xml_diff>
--- a/Destination Workbook Testing/Destination.xlsx
+++ b/Destination Workbook Testing/Destination.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20392"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2FDED7E-7C13-4961-ABC4-152A91C9E95E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817D0007-5BB6-4187-8D93-56415190924F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Team Name</t>
   </si>
@@ -32,6 +32,54 @@
   </si>
   <si>
     <t>Team Budget</t>
+  </si>
+  <si>
+    <t>Team A P1</t>
+  </si>
+  <si>
+    <t>Email A P1</t>
+  </si>
+  <si>
+    <t>Phone A P1</t>
+  </si>
+  <si>
+    <t>Budget A P1</t>
+  </si>
+  <si>
+    <t>Team A P2</t>
+  </si>
+  <si>
+    <t>Email A P2</t>
+  </si>
+  <si>
+    <t>Phone A P2</t>
+  </si>
+  <si>
+    <t>Budget A P2</t>
+  </si>
+  <si>
+    <t>Team B P1</t>
+  </si>
+  <si>
+    <t>Email B P1</t>
+  </si>
+  <si>
+    <t>Phone B P1</t>
+  </si>
+  <si>
+    <t>Budget B P1</t>
+  </si>
+  <si>
+    <t>Team B P2</t>
+  </si>
+  <si>
+    <t>Email B P2</t>
+  </si>
+  <si>
+    <t>Phone B P2</t>
+  </si>
+  <si>
+    <t>Budget B P2</t>
   </si>
 </sst>
 </file>
@@ -363,7 +411,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D5" sqref="A2:D5"/>
@@ -389,6 +437,62 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>